<commit_message>
adding better error handling
</commit_message>
<xml_diff>
--- a/inst/sample_data/simdat.xlsx
+++ b/inst/sample_data/simdat.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="scores" sheetId="1" r:id="rId1"/>
     <sheet name="map" sheetId="2" r:id="rId2"/>
+    <sheet name="frequencies" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="132">
   <si>
     <t>accession_id</t>
   </si>
@@ -407,6 +408,15 @@
   </si>
   <si>
     <t>chromosome</t>
+  </si>
+  <si>
+    <t>marker</t>
+  </si>
+  <si>
+    <t>marker_size</t>
+  </si>
+  <si>
+    <t>frequency</t>
   </si>
 </sst>
 </file>
@@ -743,7 +753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CD11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -3402,7 +3412,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3603,4 +3613,927 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2">
+        <v>147</v>
+      </c>
+      <c r="C2">
+        <v>1.5267175572519101E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3">
+        <v>149</v>
+      </c>
+      <c r="C3">
+        <v>1.01781170483461E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4">
+        <v>150</v>
+      </c>
+      <c r="C4">
+        <v>1.7811704834605601E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5">
+        <v>151</v>
+      </c>
+      <c r="C5">
+        <v>1.5267175572519101E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6">
+        <v>178</v>
+      </c>
+      <c r="C6">
+        <v>1.5267175572519101E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7">
+        <v>181</v>
+      </c>
+      <c r="C7">
+        <v>1.7811704834605601E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8">
+        <v>183</v>
+      </c>
+      <c r="C8">
+        <v>1.5267175572519101E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9">
+        <v>185</v>
+      </c>
+      <c r="C9">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10">
+        <v>143</v>
+      </c>
+      <c r="C10">
+        <v>1.7811704834605601E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11">
+        <v>149</v>
+      </c>
+      <c r="C11">
+        <v>2.5445292620865098E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12">
+        <v>152</v>
+      </c>
+      <c r="C12">
+        <v>7.63358778625954E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13">
+        <v>155</v>
+      </c>
+      <c r="C13">
+        <v>1.5267175572519101E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14">
+        <v>172</v>
+      </c>
+      <c r="C14">
+        <v>1.7811704834605601E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15">
+        <v>216</v>
+      </c>
+      <c r="C15">
+        <v>7.63358778625954E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16">
+        <v>217</v>
+      </c>
+      <c r="C16">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17">
+        <v>221</v>
+      </c>
+      <c r="C17">
+        <v>7.63358778625954E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18">
+        <v>196</v>
+      </c>
+      <c r="C18">
+        <v>7.63358778625954E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19">
+        <v>199</v>
+      </c>
+      <c r="C19">
+        <v>1.5267175572519101E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20">
+        <v>205</v>
+      </c>
+      <c r="C20">
+        <v>5.0890585241730301E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21">
+        <v>160</v>
+      </c>
+      <c r="C21">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22">
+        <v>169</v>
+      </c>
+      <c r="C22">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23">
+        <v>172</v>
+      </c>
+      <c r="C23">
+        <v>1.01781170483461E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24">
+        <v>175</v>
+      </c>
+      <c r="C24">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25">
+        <v>114</v>
+      </c>
+      <c r="C25">
+        <v>7.63358778625954E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26">
+        <v>122</v>
+      </c>
+      <c r="C26">
+        <v>1.01781170483461E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27">
+        <v>96</v>
+      </c>
+      <c r="C27">
+        <v>1.5267175572519101E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28">
+        <v>186</v>
+      </c>
+      <c r="C28">
+        <v>7.63358778625954E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29">
+        <v>190</v>
+      </c>
+      <c r="C29">
+        <v>1.7811704834605601E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30">
+        <v>202</v>
+      </c>
+      <c r="C30">
+        <v>1.5267175572519101E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31">
+        <v>205</v>
+      </c>
+      <c r="C31">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>115</v>
+      </c>
+      <c r="B32">
+        <v>139</v>
+      </c>
+      <c r="C32">
+        <v>7.63358778625954E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B33">
+        <v>145</v>
+      </c>
+      <c r="C33">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34">
+        <v>148</v>
+      </c>
+      <c r="C34">
+        <v>1.5267175572519101E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35">
+        <v>108</v>
+      </c>
+      <c r="C35">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>124</v>
+      </c>
+      <c r="B36">
+        <v>111</v>
+      </c>
+      <c r="C36">
+        <v>1.01781170483461E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>124</v>
+      </c>
+      <c r="B37">
+        <v>114</v>
+      </c>
+      <c r="C37">
+        <v>7.63358778625954E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38">
+        <v>117</v>
+      </c>
+      <c r="C38">
+        <v>1.5267175572519101E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B39">
+        <v>120</v>
+      </c>
+      <c r="C39">
+        <v>5.0890585241730301E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>104</v>
+      </c>
+      <c r="B40">
+        <v>137</v>
+      </c>
+      <c r="C40">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>104</v>
+      </c>
+      <c r="B41">
+        <v>143</v>
+      </c>
+      <c r="C41">
+        <v>1.5267175572519101E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42">
+        <v>131</v>
+      </c>
+      <c r="C42">
+        <v>1.7811704834605601E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43">
+        <v>186</v>
+      </c>
+      <c r="C43">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44">
+        <v>204</v>
+      </c>
+      <c r="C44">
+        <v>1.01781170483461E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>123</v>
+      </c>
+      <c r="B45">
+        <v>102</v>
+      </c>
+      <c r="C45">
+        <v>1.7811704834605601E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46">
+        <v>107</v>
+      </c>
+      <c r="C46">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>123</v>
+      </c>
+      <c r="B47">
+        <v>90</v>
+      </c>
+      <c r="C47">
+        <v>7.63358778625954E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48">
+        <v>92</v>
+      </c>
+      <c r="C48">
+        <v>2.03562340966921E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>123</v>
+      </c>
+      <c r="B49">
+        <v>94</v>
+      </c>
+      <c r="C49">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>117</v>
+      </c>
+      <c r="B50">
+        <v>227</v>
+      </c>
+      <c r="C50">
+        <v>1.5267175572519101E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>117</v>
+      </c>
+      <c r="B51">
+        <v>236</v>
+      </c>
+      <c r="C51">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>117</v>
+      </c>
+      <c r="B52">
+        <v>245</v>
+      </c>
+      <c r="C52">
+        <v>1.01781170483461E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53">
+        <v>181</v>
+      </c>
+      <c r="C53">
+        <v>1.5267175572519101E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>100</v>
+      </c>
+      <c r="B54">
+        <v>187</v>
+      </c>
+      <c r="C54">
+        <v>7.63358778625954E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>100</v>
+      </c>
+      <c r="B55">
+        <v>190</v>
+      </c>
+      <c r="C55">
+        <v>1.7811704834605601E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56">
+        <v>191</v>
+      </c>
+      <c r="C56">
+        <v>7.63358778625954E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>95</v>
+      </c>
+      <c r="B57">
+        <v>207</v>
+      </c>
+      <c r="C57">
+        <v>7.63358778625954E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58">
+        <v>209</v>
+      </c>
+      <c r="C58">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>95</v>
+      </c>
+      <c r="B59">
+        <v>214</v>
+      </c>
+      <c r="C59">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>114</v>
+      </c>
+      <c r="B60">
+        <v>185</v>
+      </c>
+      <c r="C60">
+        <v>7.63358778625954E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>114</v>
+      </c>
+      <c r="B61">
+        <v>188</v>
+      </c>
+      <c r="C61">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>114</v>
+      </c>
+      <c r="B62">
+        <v>189</v>
+      </c>
+      <c r="C62">
+        <v>1.5267175572519101E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63">
+        <v>192</v>
+      </c>
+      <c r="C63">
+        <v>1.5267175572519101E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>120</v>
+      </c>
+      <c r="B64">
+        <v>170</v>
+      </c>
+      <c r="C64">
+        <v>1.01781170483461E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>120</v>
+      </c>
+      <c r="B65">
+        <v>173</v>
+      </c>
+      <c r="C65">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>120</v>
+      </c>
+      <c r="B66">
+        <v>176</v>
+      </c>
+      <c r="C66">
+        <v>1.01781170483461E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>120</v>
+      </c>
+      <c r="B67">
+        <v>179</v>
+      </c>
+      <c r="C67">
+        <v>1.5267175572519101E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>97</v>
+      </c>
+      <c r="B68">
+        <v>305</v>
+      </c>
+      <c r="C68">
+        <v>1.01781170483461E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>97</v>
+      </c>
+      <c r="B69">
+        <v>308</v>
+      </c>
+      <c r="C69">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>97</v>
+      </c>
+      <c r="B70">
+        <v>314</v>
+      </c>
+      <c r="C70">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>126</v>
+      </c>
+      <c r="B71">
+        <v>300</v>
+      </c>
+      <c r="C71">
+        <v>2.2900763358778602E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>126</v>
+      </c>
+      <c r="B72">
+        <v>307</v>
+      </c>
+      <c r="C72">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>94</v>
+      </c>
+      <c r="B73">
+        <v>259</v>
+      </c>
+      <c r="C73">
+        <v>1.01781170483461E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>94</v>
+      </c>
+      <c r="B74">
+        <v>264</v>
+      </c>
+      <c r="C74">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>94</v>
+      </c>
+      <c r="B75">
+        <v>270</v>
+      </c>
+      <c r="C75">
+        <v>7.63358778625954E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>94</v>
+      </c>
+      <c r="B76">
+        <v>277</v>
+      </c>
+      <c r="C76">
+        <v>1.5267175572519101E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>94</v>
+      </c>
+      <c r="B77">
+        <v>286</v>
+      </c>
+      <c r="C77">
+        <v>1.5267175572519101E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>94</v>
+      </c>
+      <c r="B78">
+        <v>289</v>
+      </c>
+      <c r="C78">
+        <v>1.01781170483461E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>106</v>
+      </c>
+      <c r="B79">
+        <v>246</v>
+      </c>
+      <c r="C79">
+        <v>1.27226463104326E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>106</v>
+      </c>
+      <c r="B80">
+        <v>248</v>
+      </c>
+      <c r="C80">
+        <v>1.01781170483461E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>106</v>
+      </c>
+      <c r="B81">
+        <v>250</v>
+      </c>
+      <c r="C81">
+        <v>1.01781170483461E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>106</v>
+      </c>
+      <c r="B82">
+        <v>256</v>
+      </c>
+      <c r="C82">
+        <v>7.63358778625954E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>